<commit_message>
Implemented advance for days
</commit_message>
<xml_diff>
--- a/functions.xlsx
+++ b/functions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiarf\Desktop\cpp\bootstrapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiarf\Documents\GitHub\bootstrapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F1A365-6651-4D07-8B8E-16A2B41A3074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EB7FCE-73FB-4BAF-ADB4-603F2DDE652E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{D7DA6D72-5A15-4013-87E0-D24AED0AEF2B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{D7DA6D72-5A15-4013-87E0-D24AED0AEF2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,6 +428,50 @@
         <a:xfrm>
           <a:off x="0" y="12763500"/>
           <a:ext cx="10364646" cy="5353797"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>486601</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>191</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CDEBBBA-4D41-67F2-4C22-D96CB615F3EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10420350" y="12725400"/>
+          <a:ext cx="5915851" cy="1371791"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -821,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807AF91E-0D3B-411F-A339-01B8AFAB9B6E}">
   <dimension ref="A33"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -842,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796BF369-BDB9-4727-9C6A-D1AB0BD2A96D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="X79" sqref="X79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added classes to be implemented
</commit_message>
<xml_diff>
--- a/functions.xlsx
+++ b/functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiarf\Documents\GitHub\bootstrapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A51C11-F0FC-47D3-B897-2DB2944FF52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255E586C-6489-419E-B096-0003BC539D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{D7DA6D72-5A15-4013-87E0-D24AED0AEF2B}"/>
   </bookViews>
@@ -1479,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E38CA1-BBFC-4859-A4B2-B5A2F673F30B}">
   <dimension ref="A50:Z66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="Q47" sqref="Q47"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="S52" sqref="S52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,10 +1504,22 @@
       <c r="A62" t="s">
         <v>8</v>
       </c>
+      <c r="I62">
+        <f>4/365</f>
+        <v>1.0958904109589041E-2</v>
+      </c>
+      <c r="J62">
+        <f>5/365</f>
+        <v>1.3698630136986301E-2</v>
+      </c>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>9</v>
+      </c>
+      <c r="I63">
+        <f>94/365</f>
+        <v>0.25753424657534246</v>
       </c>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>